<commit_message>
added on off button and remove LCD resstor
</commit_message>
<xml_diff>
--- a/6lowPan/Gerber and BoM/Gerber and BoM/ANNA-BoM.xlsx
+++ b/6lowPan/Gerber and BoM/Gerber and BoM/ANNA-BoM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tritronik\Documents\Project\EMMA\PCB\6lowPan\Gerber and BoM\Gerber and BoM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="7710"/>
   </bookViews>
@@ -19,7 +24,7 @@
     <author>tritronik</author>
   </authors>
   <commentList>
-    <comment ref="A66" authorId="0">
+    <comment ref="A66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="218">
   <si>
     <t>Ref</t>
   </si>
@@ -574,9 +579,6 @@
     <t>R35, R34, R30, R32</t>
   </si>
   <si>
-    <t>R92, LCD-R1</t>
-  </si>
-  <si>
     <t>LED1, LED2</t>
   </si>
   <si>
@@ -677,6 +679,24 @@
   </si>
   <si>
     <t>ANT1, ANT2</t>
+  </si>
+  <si>
+    <t>R92</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>PUSH SWITCH</t>
+  </si>
+  <si>
+    <t>6pin 2.54mm spacing locked push switch (with white cap)</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>cap</t>
   </si>
 </sst>
 </file>
@@ -773,6 +793,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -820,7 +843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -855,7 +878,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1064,15 +1087,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
@@ -1096,7 +1121,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1113,7 +1138,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1147,7 +1172,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -1164,7 +1189,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -1263,7 +1288,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>33</v>
@@ -1279,7 +1304,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
@@ -1296,7 +1321,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
@@ -1333,7 +1358,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
@@ -1384,7 +1409,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
@@ -1401,7 +1426,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
         <v>50</v>
@@ -1418,7 +1443,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
         <v>55</v>
@@ -1435,7 +1460,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
@@ -1452,7 +1477,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s">
         <v>58</v>
@@ -1472,7 +1497,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B24" t="s">
         <v>50</v>
@@ -1509,7 +1534,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
@@ -1526,7 +1551,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B27" t="s">
         <v>64</v>
@@ -1543,7 +1568,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B28" t="s">
         <v>66</v>
@@ -1560,7 +1585,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B29" t="s">
         <v>66</v>
@@ -1577,7 +1602,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B30" t="s">
         <v>70</v>
@@ -1651,7 +1676,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B34" t="s">
         <v>66</v>
@@ -1702,7 +1727,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s">
         <v>66</v>
@@ -1719,7 +1744,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B38" t="s">
         <v>66</v>
@@ -1770,7 +1795,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B41" t="s">
         <v>92</v>
@@ -1855,7 +1880,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
@@ -1872,7 +1897,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
@@ -1940,7 +1965,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="B51" t="s">
         <v>66</v>
@@ -1957,7 +1982,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52" t="s">
         <v>66</v>
@@ -2028,7 +2053,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B56" t="s">
         <v>117</v>
@@ -2065,7 +2090,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B58" t="s">
         <v>123</v>
@@ -2122,7 +2147,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C61" t="s">
         <v>132</v>
@@ -2213,7 +2238,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B66" t="s">
         <v>150</v>
@@ -2233,7 +2258,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B67" t="s">
         <v>153</v>
@@ -2250,7 +2275,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B68" t="s">
         <v>156</v>
@@ -2270,7 +2295,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B69" t="s">
         <v>158</v>
@@ -2352,7 +2377,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B74" t="s">
         <v>50</v>
@@ -2364,6 +2389,31 @@
         <v>172</v>
       </c>
       <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>213</v>
+      </c>
+      <c r="B75" t="s">
+        <v>214</v>
+      </c>
+      <c r="C75" t="s">
+        <v>215</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E76" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F76">
         <v>1</v>
       </c>
     </row>
@@ -2395,9 +2445,11 @@
     <hyperlink ref="E17" r:id="rId24"/>
     <hyperlink ref="E2" r:id="rId25"/>
     <hyperlink ref="E11" r:id="rId26"/>
+    <hyperlink ref="E75" r:id="rId27"/>
+    <hyperlink ref="E76" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId27"/>
-  <legacyDrawing r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId29"/>
+  <legacyDrawing r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
routing mcb-enhancer, not DRC/ERC-ed yet
</commit_message>
<xml_diff>
--- a/6lowPan/Gerber and BoM/Gerber and BoM/ANNA-BoM.xlsx
+++ b/6lowPan/Gerber and BoM/Gerber and BoM/ANNA-BoM.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="227">
   <si>
     <t>Ref</t>
   </si>
@@ -697,6 +697,33 @@
   </si>
   <si>
     <t>cap</t>
+  </si>
+  <si>
+    <t>ACCESSORIES</t>
+  </si>
+  <si>
+    <t>SCT-013</t>
+  </si>
+  <si>
+    <t>Current sensor with RJ11 jack</t>
+  </si>
+  <si>
+    <t>LCD 2.4inch</t>
+  </si>
+  <si>
+    <t>LCD TFT with touch capabilities 2.4inch</t>
+  </si>
+  <si>
+    <t>alibaba link</t>
+  </si>
+  <si>
+    <t>aliexpress link</t>
+  </si>
+  <si>
+    <t>GPRS antenna</t>
+  </si>
+  <si>
+    <t>PCB antenna for SIM900 GPRS</t>
   </si>
 </sst>
 </file>
@@ -742,7 +769,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -761,6 +788,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -775,13 +808,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1087,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,6 +2448,53 @@
         <v>217</v>
       </c>
       <c r="F76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>219</v>
+      </c>
+      <c r="C78" t="s">
+        <v>220</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>221</v>
+      </c>
+      <c r="C79" t="s">
+        <v>222</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>225</v>
+      </c>
+      <c r="C80" t="s">
+        <v>226</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F80">
         <v>1</v>
       </c>
     </row>
@@ -2447,9 +2528,12 @@
     <hyperlink ref="E11" r:id="rId26"/>
     <hyperlink ref="E75" r:id="rId27"/>
     <hyperlink ref="E76" r:id="rId28"/>
+    <hyperlink ref="E78" r:id="rId29"/>
+    <hyperlink ref="E79" r:id="rId30"/>
+    <hyperlink ref="E80" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId29"/>
-  <legacyDrawing r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId32"/>
+  <legacyDrawing r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>